<commit_message>
se agregó instalador de ghostcript
</commit_message>
<xml_diff>
--- a/To.Rpa.AppCTS/CTS/WORKSPACE/RETAZOS/4023/PLANTILLA/Plantilla abono CTS - 4023.xlsx
+++ b/To.Rpa.AppCTS/CTS/WORKSPACE/RETAZOS/4023/PLANTILLA/Plantilla abono CTS - 4023.xlsx
@@ -1182,8 +1182,8 @@
       <x:c r="C5" s="10" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="D5" s="48">
-        <x:v>20159473148</x:v>
+      <x:c r="D5" s="48" t="n">
+        <x:v>20512868046</x:v>
       </x:c>
       <x:c r="E5" s="55"/>
       <x:c r="G5" s="10" t="s">
@@ -1194,8 +1194,8 @@
       <x:c r="J5" s="13" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="K5" s="29">
-        <x:v>3968</x:v>
+      <x:c r="K5" s="29" t="n">
+        <x:v>4023</x:v>
       </x:c>
       <x:c r="L5" s="21" t="s">
         <x:v>29</x:v>
@@ -1213,22 +1213,22 @@
       <x:c r="C7" s="10" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="D7" s="48" t="s">
-        <x:v>39</x:v>
+      <x:c r="D7" s="48" t="n">
+        <x:v>MAY</x:v>
       </x:c>
       <x:c r="E7" s="55"/>
       <x:c r="F7" s="5"/>
       <x:c r="G7" s="10" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="H7" s="27">
+      <x:c r="H7" s="27" t="n">
         <x:v>2018</x:v>
       </x:c>
       <x:c r="J7" s="13" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="K7" s="30" t="s">
-        <x:v>37</x:v>
+      <x:c r="K7" s="30" t="n">
+        <x:v>DOL</x:v>
       </x:c>
       <x:c r="L7" s="1"/>
     </x:row>
@@ -1485,27 +1485,27 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C25" s="35" t="n">
-        <x:v>RIGOBERTO ANGEL MILLA QUINONEZ</x:v>
+        <x:v>RIGOBERTO ANOEL NIILLA OUINONEZ _</x:v>
       </x:c>
       <x:c r="D25" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
       <x:c r="E25" s="36" t="n">
-        <x:v>32793730</x:v>
+        <x:v>332793730</x:v>
       </x:c>
       <x:c r="F25" s="35" t="n">
-        <x:v>000976730496</x:v>
-      </x:c>
-      <x:c r="G25" s="40" t="n">
+        <x:v>000975730495</x:v>
+      </x:c>
+      <x:c r="G25" s="40" t="str">
         <x:f>+$K$7</x:f>
-        <x:v>ﬁfﬁuauummuui</x:v>
+        <x:v>SOL</x:v>
       </x:c>
       <x:c r="H25" s="35" t="n">
         <x:v>247.45</x:v>
       </x:c>
       <x:c r="I25" s="40" t="n">
         <x:f>+$K$7</x:f>
-        <x:v>SOL</x:v>
+        <x:v>i</x:v>
       </x:c>
       <x:c r="J25" s="42" t="n">
         <x:v>18,951.59</x:v>
@@ -1523,7 +1523,7 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="C26" s="35" t="n">
-        <x:v>MM-</x:v>
+        <x:v>GUILLERMO ANGEL RUMICHE ORSESOZO _</x:v>
       </x:c>
       <x:c r="D26" s="32" t="s">
         <x:v>38</x:v>
@@ -1532,21 +1532,21 @@
         <x:v>32948694</x:v>
       </x:c>
       <x:c r="F26" s="35" t="n">
-        <x:v>000611398133</x:v>
-      </x:c>
-      <x:c r="G26" s="40" t="n">
+        <x:v>000511393133</x:v>
+      </x:c>
+      <x:c r="G26" s="40" t="str">
         <x:f t="shared" ref="G26:G89" si="0">+$K$7</x:f>
-        <x:v>W$ﬁﬁsAL</x:v>
+        <x:v>SOL</x:v>
       </x:c>
       <x:c r="H26" s="35" t="n">
         <x:v>171.14</x:v>
       </x:c>
       <x:c r="I26" s="40" t="n">
         <x:f t="shared" ref="I26:I89" si="1">+$K$7</x:f>
-        <x:v>SOL</x:v>
+        <x:v>L”:</x:v>
       </x:c>
       <x:c r="J26" s="42" t="n">
-        <x:v>10,707.94</x:v>
+        <x:v>19,707,94</x:v>
       </x:c>
       <x:c r="K26" s="43" t="n">
         <x:v>SOL</x:v>
@@ -1561,7 +1561,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="C27" s="35" t="n">
-        <x:v>GUILLERMO ANGEL RUMICHE ORBEGOZO</x:v>
+        <x:v>SANTOS ROEL SALAS GIL __ I</x:v>
       </x:c>
       <x:c r="D27" s="32" t="s">
         <x:v>38</x:v>
@@ -1570,7 +1570,7 @@
         <x:v>32966945</x:v>
       </x:c>
       <x:c r="F27" s="35" t="n">
-        <x:v>000978730460</x:v>
+        <x:v>000975730455</x:v>
       </x:c>
       <x:c r="G27" s="40" t="str">
         <x:f t="shared" si="0"/>
@@ -1581,7 +1581,7 @@
       </x:c>
       <x:c r="I27" s="40" t="n">
         <x:f t="shared" si="1"/>
-        <x:v>SOL</x:v>
+        <x:v>r~\§(- _. ,..‘.-.- .</x:v>
       </x:c>
       <x:c r="J27" s="42" t="n">
         <x:v>17,259.74</x:v>
@@ -1599,16 +1599,16 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="C28" s="35" t="n">
-        <x:v>SANTOS ROEL SALAS GIL</x:v>
+        <x:v>NESTOR ANTONIO MONTES MEDINA</x:v>
       </x:c>
       <x:c r="D28" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
       <x:c r="E28" s="36" t="n">
-        <x:v>32973962</x:v>
+        <x:v>332973952</x:v>
       </x:c>
       <x:c r="F28" s="35" t="n">
-        <x:v>000606178252</x:v>
+        <x:v>000555175252</x:v>
       </x:c>
       <x:c r="G28" s="40" t="str">
         <x:f t="shared" si="0"/>
@@ -1619,10 +1619,10 @@
       </x:c>
       <x:c r="I28" s="40" t="n">
         <x:f t="shared" si="1"/>
-        <x:v>SOL</x:v>
+        <x:v>émmﬁﬁﬁa-g‘qﬁfﬂ; a. an F9 _. ‘ “3‘...</x:v>
       </x:c>
       <x:c r="J28" s="42" t="n">
-        <x:v>43,904.95</x:v>
+        <x:v>43,604.95</x:v>
       </x:c>
       <x:c r="K28" s="43" t="n">
         <x:v>SOL</x:v>
@@ -1637,7 +1637,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="C29" s="35" t="n">
-        <x:v>NESTOR ANTONIO MONTES MEDINA</x:v>
+        <x:v>AOALSERTO RUIZ SANOOVAL I</x:v>
       </x:c>
       <x:c r="D29" s="32" t="s">
         <x:v>38</x:v>
@@ -1646,21 +1646,21 @@
         <x:v>32913099</x:v>
       </x:c>
       <x:c r="F29" s="35" t="n">
-        <x:v>000978669559</x:v>
+        <x:v>001975559559</x:v>
       </x:c>
       <x:c r="G29" s="40" t="str">
         <x:f t="shared" si="0"/>
         <x:v>SOL</x:v>
       </x:c>
       <x:c r="H29" s="35" t="n">
-        <x:v>344.91</x:v>
+        <x:v>344.01</x:v>
       </x:c>
       <x:c r="I29" s="40" t="n">
         <x:f t="shared" si="1"/>
-        <x:v>SOL</x:v>
+        <x:v>_ . _. ..._ ._ 14-23, '1.-</x:v>
       </x:c>
       <x:c r="J29" s="42" t="n">
-        <x:v>13,114.05</x:v>
+        <x:v>13,114.09</x:v>
       </x:c>
       <x:c r="K29" s="43" t="n">
         <x:v>SOL</x:v>
@@ -1675,27 +1675,27 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C30" s="35" t="n">
-        <x:v>ADALBERTO RUIZ SANDOVAL</x:v>
+        <x:v>ILUl-S ALBERTO CHINGA RAMOS</x:v>
       </x:c>
       <x:c r="D30" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
       <x:c r="E30" s="36" t="n">
-        <x:v>15641527</x:v>
+        <x:v>15341527</x:v>
       </x:c>
       <x:c r="F30" s="35" t="n">
-        <x:v>000978869826</x:v>
+        <x:v>000975559825</x:v>
       </x:c>
       <x:c r="G30" s="40" t="str">
         <x:f t="shared" si="0"/>
         <x:v>SOL</x:v>
       </x:c>
       <x:c r="H30" s="35" t="n">
-        <x:v>681.80</x:v>
+        <x:v>031.30</x:v>
       </x:c>
       <x:c r="I30" s="40" t="n">
         <x:f t="shared" si="1"/>
-        <x:v>SOL</x:v>
+        <x:v>. .- '</x:v>
       </x:c>
       <x:c r="J30" s="42" t="n">
         <x:v>39,972.92</x:v>
@@ -1713,16 +1713,16 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="C31" s="35" t="n">
-        <x:v>LUIS ALBERTO CHINGA RAMOS</x:v>
+        <x:v>JUAN MANUEL MONTALVAN GUERRERO</x:v>
       </x:c>
       <x:c r="D31" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
       <x:c r="E31" s="36" t="n">
-        <x:v>32962571</x:v>
+        <x:v>32952571</x:v>
       </x:c>
       <x:c r="F31" s="35" t="n">
-        <x:v>000963861476</x:v>
+        <x:v>000953551475</x:v>
       </x:c>
       <x:c r="G31" s="40" t="str">
         <x:f t="shared" si="0"/>
@@ -1733,7 +1733,7 @@
       </x:c>
       <x:c r="I31" s="40" t="n">
         <x:f t="shared" si="1"/>
-        <x:v>SOL</x:v>
+        <x:v>30L</x:v>
       </x:c>
       <x:c r="J31" s="42" t="n">
         <x:v>6,490.68</x:v>
@@ -1751,7 +1751,7 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="C32" s="35" t="n">
-        <x:v>JUAN MANUEL MONTALVAN GUERRERO</x:v>
+        <x:v>ROBERTO ANDRES VILLANUEVA TOLENTINO</x:v>
       </x:c>
       <x:c r="D32" s="32" t="s">
         <x:v>38</x:v>
@@ -1760,21 +1760,21 @@
         <x:v>32319397</x:v>
       </x:c>
       <x:c r="F32" s="35" t="n">
-        <x:v>000948137616</x:v>
+        <x:v>000943137515</x:v>
       </x:c>
       <x:c r="G32" s="40" t="str">
         <x:f t="shared" si="0"/>
         <x:v>SOL</x:v>
       </x:c>
       <x:c r="H32" s="35" t="n">
-        <x:v>41.64</x:v>
+        <x:v>41.34</x:v>
       </x:c>
       <x:c r="I32" s="40" t="n">
         <x:f t="shared" si="1"/>
         <x:v>SOL</x:v>
       </x:c>
       <x:c r="J32" s="42" t="n">
-        <x:v>6,950.58</x:v>
+        <x:v>6,950.53</x:v>
       </x:c>
       <x:c r="K32" s="43" t="n">
         <x:v>SOL</x:v>
@@ -1789,16 +1789,16 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="C33" s="35" t="n">
-        <x:v>ROBERTO ANDRES VILLANUEVA TOLENTINO</x:v>
+        <x:v>OSCAR JAIME CABALLERO PEREZ</x:v>
       </x:c>
       <x:c r="D33" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
       <x:c r="E33" s="36" t="n">
-        <x:v>41034075</x:v>
+        <x:v>41034975</x:v>
       </x:c>
       <x:c r="F33" s="35" t="n">
-        <x:v>000978730429</x:v>
+        <x:v>000973730429</x:v>
       </x:c>
       <x:c r="G33" s="40" t="str">
         <x:f t="shared" si="0"/>
@@ -1809,10 +1809,10 @@
       </x:c>
       <x:c r="I33" s="40" t="n">
         <x:f t="shared" si="1"/>
-        <x:v>SOL</x:v>
+        <x:v>_ SOL</x:v>
       </x:c>
       <x:c r="J33" s="42" t="n">
-        <x:v>8,987.70</x:v>
+        <x:v>3,987.70</x:v>
       </x:c>
       <x:c r="K33" s="43" t="n">
         <x:v>SOL</x:v>
@@ -1827,7 +1827,7 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="C34" s="35" t="n">
-        <x:v>OSCAR JAIME CABALLERO PEREZ</x:v>
+        <x:v>MAXIIMO ROBERTO FLORES OSORIO</x:v>
       </x:c>
       <x:c r="D34" s="32" t="s">
         <x:v>38</x:v>
@@ -1836,21 +1836,21 @@
         <x:v>09576136</x:v>
       </x:c>
       <x:c r="F34" s="35" t="n">
-        <x:v>000976759010</x:v>
+        <x:v>100975759015</x:v>
       </x:c>
       <x:c r="G34" s="40" t="str">
         <x:f t="shared" si="0"/>
         <x:v>SOL</x:v>
       </x:c>
       <x:c r="H34" s="35" t="n">
-        <x:v>240.83</x:v>
+        <x:v>240.33</x:v>
       </x:c>
       <x:c r="I34" s="40" t="n">
         <x:f t="shared" si="1"/>
         <x:v>SOL</x:v>
       </x:c>
       <x:c r="J34" s="42" t="n">
-        <x:v>17,255.02</x:v>
+        <x:v>17,25502</x:v>
       </x:c>
       <x:c r="K34" s="43" t="n">
         <x:v>SOL</x:v>
@@ -1865,16 +1865,16 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="C35" s="35" t="n">
-        <x:v>MAXIMO ROBERTO FLORES OSORIO</x:v>
+        <x:v>WILLtAM EUSEBIO MUNOZ FERNANDEZ</x:v>
       </x:c>
       <x:c r="D35" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
       <x:c r="E35" s="36" t="n">
-        <x:v>32961651</x:v>
+        <x:v>32991551</x:v>
       </x:c>
       <x:c r="F35" s="35" t="n">
-        <x:v>000971841527</x:v>
+        <x:v>000971541527</x:v>
       </x:c>
       <x:c r="G35" s="40" t="str">
         <x:f t="shared" si="0"/>
@@ -1888,7 +1888,7 @@
         <x:v>SOL</x:v>
       </x:c>
       <x:c r="J35" s="42" t="n">
-        <x:v>7,246.29</x:v>
+        <x:v>7,245.29</x:v>
       </x:c>
       <x:c r="K35" s="43" t="n">
         <x:v>SOL</x:v>
@@ -1903,7 +1903,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="C36" s="35" t="n">
-        <x:v>[WILLIAM EUSEBIO MUNOZ FERNANDEZ</x:v>
+        <x:v>FREDDY CESARCHAVEZ DE LA CRUZ</x:v>
       </x:c>
       <x:c r="D36" s="32" t="s">
         <x:v>38</x:v>
@@ -1912,7 +1912,7 @@
         <x:v>32940729</x:v>
       </x:c>
       <x:c r="F36" s="35" t="n">
-        <x:v>000956529062</x:v>
+        <x:v>000955529052</x:v>
       </x:c>
       <x:c r="G36" s="40" t="str">
         <x:f t="shared" si="0"/>
@@ -1923,7 +1923,7 @@
       </x:c>
       <x:c r="I36" s="40" t="n">
         <x:f t="shared" si="1"/>
-        <x:v>SOL</x:v>
+        <x:v>50.1-</x:v>
       </x:c>
       <x:c r="J36" s="42" t="n">
         <x:v>7,507.79</x:v>
@@ -1941,16 +1941,16 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="C37" s="35" t="n">
-        <x:v>FREDDY CESAR CHAVEZ DE LA CRUZ</x:v>
+        <x:v>JUANFRANCISCO MEDINA MONCADA</x:v>
       </x:c>
       <x:c r="D37" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
       <x:c r="E37" s="36" t="n">
-        <x:v>32730152</x:v>
+        <x:v>32739132</x:v>
       </x:c>
       <x:c r="F37" s="35" t="n">
-        <x:v>000964325039</x:v>
+        <x:v>000954325039</x:v>
       </x:c>
       <x:c r="G37" s="40" t="str">
         <x:f t="shared" si="0"/>
@@ -1964,10 +1964,10 @@
         <x:v>SOL</x:v>
       </x:c>
       <x:c r="J37" s="42" t="n">
-        <x:v>12,446.79</x:v>
+        <x:v>12,449.79</x:v>
       </x:c>
       <x:c r="K37" s="43" t="n">
-        <x:v>SOL</x:v>
+        <x:v>50L . .</x:v>
       </x:c>
       <x:c r="M37" s="22" t="str">
         <x:f t="shared" si="2"/>
@@ -1979,7 +1979,7 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="C38" s="35" t="n">
-        <x:v>JUAN FRANCISCO MEDINA MONCADA</x:v>
+        <x:v>MIGUEL ANGEL LLONTOP OUIROZ</x:v>
       </x:c>
       <x:c r="D38" s="32" t="s">
         <x:v>38</x:v>
@@ -1988,24 +1988,24 @@
         <x:v>42911460</x:v>
       </x:c>
       <x:c r="F38" s="35" t="n">
-        <x:v>000964325020</x:v>
+        <x:v>000954325020</x:v>
       </x:c>
       <x:c r="G38" s="40" t="str">
         <x:f t="shared" si="0"/>
         <x:v>SOL</x:v>
       </x:c>
       <x:c r="H38" s="35" t="n">
-        <x:v>14.78</x:v>
+        <x:v>14.73</x:v>
       </x:c>
       <x:c r="I38" s="40" t="n">
         <x:f t="shared" si="1"/>
         <x:v>SOL</x:v>
       </x:c>
       <x:c r="J38" s="42" t="n">
-        <x:v>7,818.11</x:v>
+        <x:v>7,919.11</x:v>
       </x:c>
       <x:c r="K38" s="43" t="n">
-        <x:v>SOL</x:v>
+        <x:v>soL</x:v>
       </x:c>
       <x:c r="M38" s="22" t="str">
         <x:f t="shared" si="2"/>
@@ -2017,16 +2017,16 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="C39" s="35" t="n">
-        <x:v>MIGUEL ANGEL LLONTOP QUIROZ</x:v>
+        <x:v>CORNELIO SEBASTIAN NEYRA OUISPE</x:v>
       </x:c>
       <x:c r="D39" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
       <x:c r="E39" s="36" t="n">
-        <x:v>03490874</x:v>
+        <x:v>03490374</x:v>
       </x:c>
       <x:c r="F39" s="35" t="n">
-        <x:v>000993076548</x:v>
+        <x:v>000099375545</x:v>
       </x:c>
       <x:c r="G39" s="40" t="str">
         <x:f t="shared" si="0"/>
@@ -2055,16 +2055,16 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="C40" s="35" t="n">
-        <x:v>CORNELIO SEBASTIAN NEYRA QUISPE</x:v>
+        <x:v>.. JOSE LUIS QUEREVALU SAAVEORA</x:v>
       </x:c>
       <x:c r="D40" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
       <x:c r="E40" s="36" t="n">
-        <x:v>42964776</x:v>
+        <x:v>04296476</x:v>
       </x:c>
       <x:c r="F40" s="35" t="n">
-        <x:v>000976984269</x:v>
+        <x:v>950975954259</x:v>
       </x:c>
       <x:c r="G40" s="40" t="str">
         <x:f t="shared" si="0"/>
@@ -2078,7 +2078,7 @@
         <x:v>SOL</x:v>
       </x:c>
       <x:c r="J40" s="42" t="n">
-        <x:v>17,109.80</x:v>
+        <x:v>17,109.90</x:v>
       </x:c>
       <x:c r="K40" s="43" t="n">
         <x:v>SOL</x:v>
@@ -2093,30 +2093,30 @@
         <x:v>17</x:v>
       </x:c>
       <x:c r="C41" s="35" t="n">
-        <x:v>JOSE LUIS QUEREVALU SAAVEDRA</x:v>
+        <x:v>RICARDO PERCY LA ROSA BUENOIA</x:v>
       </x:c>
       <x:c r="D41" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
       <x:c r="E41" s="36" t="n">
-        <x:v>32116039</x:v>
+        <x:v>32113039</x:v>
       </x:c>
       <x:c r="F41" s="35" t="n">
-        <x:v>000606369562</x:v>
+        <x:v>000505359552</x:v>
       </x:c>
       <x:c r="G41" s="40" t="str">
         <x:f t="shared" si="0"/>
         <x:v>SOL</x:v>
       </x:c>
       <x:c r="H41" s="35" t="n">
-        <x:v>15.62</x:v>
+        <x:v>15.02</x:v>
       </x:c>
       <x:c r="I41" s="40" t="n">
         <x:f t="shared" si="1"/>
         <x:v>SOL</x:v>
       </x:c>
       <x:c r="J41" s="42" t="n">
-        <x:v>30,781.04</x:v>
+        <x:v>30,701.04</x:v>
       </x:c>
       <x:c r="K41" s="43" t="n">
         <x:v>SOL</x:v>
@@ -2130,9 +2130,7 @@
       <x:c r="B42" s="9">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="C42" s="35" t="n">
-        <x:v>RICARDO PERCY LA ROSA BUENDIA</x:v>
-      </x:c>
+      <x:c r="C42" s="35"/>
       <x:c r="D42" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
@@ -2142,14 +2140,16 @@
         <x:f t="shared" si="0"/>
         <x:v>SOL</x:v>
       </x:c>
-      <x:c r="H42" s="35"/>
+      <x:c r="H42" s="35" t="n">
+        <x:v>2-3... .1...</x:v>
+      </x:c>
       <x:c r="I42" s="40" t="n">
         <x:f t="shared" si="1"/>
-        <x:v>SOL</x:v>
+        <x:v>' SOL __</x:v>
       </x:c>
       <x:c r="J42" s="42"/>
-      <x:c r="K42" s="43" t="s">
-        <x:v>37</x:v>
+      <x:c r="K42" s="43" t="n">
+        <x:v>...-.—-..—-.W_-_--—w-</x:v>
       </x:c>
       <x:c r="M42" s="22" t="str">
         <x:f t="shared" si="2"/>
@@ -2188,34 +2188,24 @@
       <x:c r="B44" s="9">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="C44" s="35" t="n">
-        <x:v>_________________________-———-—————-——---</x:v>
-      </x:c>
+      <x:c r="C44" s="35"/>
       <x:c r="D44" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="E44" s="36" t="n">
-        <x:v>32985941</x:v>
-      </x:c>
-      <x:c r="F44" s="35" t="n">
-        <x:v>000679607668</x:v>
-      </x:c>
-      <x:c r="G44" s="40" t="n">
+      <x:c r="E44" s="36"/>
+      <x:c r="F44" s="35"/>
+      <x:c r="G44" s="40" t="str">
         <x:f t="shared" si="0"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="H44" s="35" t="n">
-        <x:v>343.00</x:v>
-      </x:c>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="H44" s="35"/>
       <x:c r="I44" s="40" t="n">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="J44" s="42" t="n">
-        <x:v>3,600.01</x:v>
-      </x:c>
-      <x:c r="K44" s="43" t="n">
-        <x:v>SOL</x:v>
+        <x:v>ISQL .</x:v>
+      </x:c>
+      <x:c r="J44" s="42"/>
+      <x:c r="K44" s="43" t="s">
+        <x:v>37</x:v>
       </x:c>
       <x:c r="M44" s="22" t="str">
         <x:f t="shared" si="2"/>
@@ -2226,34 +2216,24 @@
       <x:c r="B45" s="9">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="C45" s="35" t="n">
-        <x:v>MICHEL IVAN PINEDO VERA</x:v>
-      </x:c>
+      <x:c r="C45" s="35"/>
       <x:c r="D45" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="E45" s="36" t="n">
-        <x:v>32934032</x:v>
-      </x:c>
-      <x:c r="F45" s="35" t="n">
-        <x:v>000838594930</x:v>
-      </x:c>
-      <x:c r="G45" s="40" t="n">
+      <x:c r="E45" s="36"/>
+      <x:c r="F45" s="35"/>
+      <x:c r="G45" s="40" t="str">
         <x:f t="shared" si="0"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="H45" s="35" t="n">
-        <x:v>249.01</x:v>
-      </x:c>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="H45" s="35"/>
       <x:c r="I45" s="40" t="n">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="J45" s="42" t="n">
-        <x:v>33,607.43</x:v>
-      </x:c>
-      <x:c r="K45" s="43" t="n">
-        <x:v>SOL</x:v>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="J45" s="42"/>
+      <x:c r="K45" s="43" t="s">
+        <x:v>37</x:v>
       </x:c>
       <x:c r="M45" s="22" t="str">
         <x:f t="shared" si="2"/>
@@ -2264,34 +2244,24 @@
       <x:c r="B46" s="9">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="C46" s="35" t="n">
-        <x:v>JAIME DAVID SAIRITUPAC EGUSQUIZA</x:v>
-      </x:c>
+      <x:c r="C46" s="35"/>
       <x:c r="D46" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="E46" s="36" t="n">
-        <x:v>40229366</x:v>
-      </x:c>
-      <x:c r="F46" s="35" t="n">
-        <x:v>000679576576</x:v>
-      </x:c>
-      <x:c r="G46" s="40" t="n">
+      <x:c r="E46" s="36"/>
+      <x:c r="F46" s="35"/>
+      <x:c r="G46" s="40" t="str">
         <x:f t="shared" si="0"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="H46" s="35" t="n">
-        <x:v>328.59</x:v>
-      </x:c>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="H46" s="35"/>
       <x:c r="I46" s="40" t="n">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="J46" s="42" t="n">
-        <x:v>1,040.00</x:v>
-      </x:c>
-      <x:c r="K46" s="43" t="n">
-        <x:v>SOL</x:v>
+        <x:v>50L</x:v>
+      </x:c>
+      <x:c r="J46" s="42"/>
+      <x:c r="K46" s="43" t="s">
+        <x:v>37</x:v>
       </x:c>
       <x:c r="M46" s="22" t="str">
         <x:f t="shared" si="2"/>
@@ -2302,34 +2272,24 @@
       <x:c r="B47" s="9">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="C47" s="35" t="n">
-        <x:v>CLEVER ALCIDES GARCIA SAAVEDRA</x:v>
-      </x:c>
+      <x:c r="C47" s="35"/>
       <x:c r="D47" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="E47" s="36" t="n">
-        <x:v>25738682</x:v>
-      </x:c>
-      <x:c r="F47" s="35" t="n">
-        <x:v>000641545963</x:v>
-      </x:c>
-      <x:c r="G47" s="40" t="n">
+      <x:c r="E47" s="36"/>
+      <x:c r="F47" s="35"/>
+      <x:c r="G47" s="40" t="str">
         <x:f t="shared" si="0"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="H47" s="35" t="n">
-        <x:v>104.86</x:v>
-      </x:c>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="H47" s="35"/>
       <x:c r="I47" s="40" t="n">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="J47" s="42" t="n">
-        <x:v>25,391.81</x:v>
-      </x:c>
-      <x:c r="K47" s="43" t="n">
-        <x:v>SOL</x:v>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="J47" s="42"/>
+      <x:c r="K47" s="43" t="s">
+        <x:v>37</x:v>
       </x:c>
       <x:c r="M47" s="22" t="str">
         <x:f t="shared" si="2"/>
@@ -2340,34 +2300,24 @@
       <x:c r="B48" s="9">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="C48" s="35" t="n">
-        <x:v>BILLY HERNAN GUANILO ESPINOZA</x:v>
-      </x:c>
+      <x:c r="C48" s="35"/>
       <x:c r="D48" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="E48" s="36" t="n">
-        <x:v>32960627</x:v>
-      </x:c>
-      <x:c r="F48" s="35" t="n">
-        <x:v>000669431656</x:v>
-      </x:c>
-      <x:c r="G48" s="40" t="n">
+      <x:c r="E48" s="36"/>
+      <x:c r="F48" s="35"/>
+      <x:c r="G48" s="40" t="str">
         <x:f t="shared" si="0"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="H48" s="35" t="n">
-        <x:v>444.02</x:v>
-      </x:c>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="H48" s="35"/>
       <x:c r="I48" s="40" t="n">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="J48" s="42" t="n">
-        <x:v>4,625.00</x:v>
-      </x:c>
-      <x:c r="K48" s="43" t="n">
-        <x:v>SOL</x:v>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="J48" s="42"/>
+      <x:c r="K48" s="43" t="s">
+        <x:v>37</x:v>
       </x:c>
       <x:c r="M48" s="22" t="str">
         <x:f t="shared" si="2"/>
@@ -2378,34 +2328,24 @@
       <x:c r="B49" s="9">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="C49" s="35" t="n">
-        <x:v>LENIN JOSE LUIS LA ROSA CRUZ</x:v>
-      </x:c>
+      <x:c r="C49" s="35"/>
       <x:c r="D49" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="E49" s="36" t="n">
-        <x:v>40275186</x:v>
-      </x:c>
-      <x:c r="F49" s="35" t="n">
-        <x:v>000596060573</x:v>
-      </x:c>
-      <x:c r="G49" s="40" t="n">
+      <x:c r="E49" s="36"/>
+      <x:c r="F49" s="35"/>
+      <x:c r="G49" s="40" t="str">
         <x:f t="shared" si="0"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="H49" s="35" t="n">
-        <x:v>445.12</x:v>
-      </x:c>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="H49" s="35"/>
       <x:c r="I49" s="40" t="n">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="J49" s="42" t="n">
-        <x:v>1,827.72</x:v>
-      </x:c>
-      <x:c r="K49" s="43" t="n">
-        <x:v>SOL</x:v>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="J49" s="42"/>
+      <x:c r="K49" s="43" t="s">
+        <x:v>37</x:v>
       </x:c>
       <x:c r="M49" s="22" t="str">
         <x:f t="shared" si="2"/>
@@ -2416,34 +2356,24 @@
       <x:c r="B50" s="9">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="C50" s="35" t="n">
-        <x:v>CARLOS HERMOGENES MARTINEZ HERNANDEZ</x:v>
-      </x:c>
+      <x:c r="C50" s="35"/>
       <x:c r="D50" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="E50" s="36" t="n">
-        <x:v>16679988</x:v>
-      </x:c>
-      <x:c r="F50" s="35" t="n">
-        <x:v>000674162926</x:v>
-      </x:c>
-      <x:c r="G50" s="40" t="n">
+      <x:c r="E50" s="36"/>
+      <x:c r="F50" s="35"/>
+      <x:c r="G50" s="40" t="str">
         <x:f t="shared" si="0"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="H50" s="35" t="n">
-        <x:v>10.72</x:v>
-      </x:c>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="H50" s="35"/>
       <x:c r="I50" s="40" t="n">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="J50" s="42" t="n">
-        <x:v>3268.06</x:v>
-      </x:c>
-      <x:c r="K50" s="43" t="n">
-        <x:v>SOL</x:v>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="J50" s="42"/>
+      <x:c r="K50" s="43" t="s">
+        <x:v>37</x:v>
       </x:c>
       <x:c r="M50" s="22" t="str">
         <x:f t="shared" si="2"/>
@@ -2454,34 +2384,24 @@
       <x:c r="B51" s="9">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="C51" s="35" t="n">
-        <x:v>BALTAZAR PISFIL CUSTODIO</x:v>
-      </x:c>
+      <x:c r="C51" s="35"/>
       <x:c r="D51" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="E51" s="36" t="n">
-        <x:v>08593828</x:v>
-      </x:c>
-      <x:c r="F51" s="35" t="n">
-        <x:v>000622560060</x:v>
-      </x:c>
-      <x:c r="G51" s="40" t="n">
+      <x:c r="E51" s="36"/>
+      <x:c r="F51" s="35"/>
+      <x:c r="G51" s="40" t="str">
         <x:f t="shared" si="0"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="H51" s="35" t="n">
-        <x:v>262.83</x:v>
-      </x:c>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="H51" s="35"/>
       <x:c r="I51" s="40" t="n">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="J51" s="42" t="n">
-        <x:v>964.00</x:v>
-      </x:c>
-      <x:c r="K51" s="43" t="n">
-        <x:v>SOL</x:v>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="J51" s="42"/>
+      <x:c r="K51" s="43" t="s">
+        <x:v>37</x:v>
       </x:c>
       <x:c r="M51" s="22" t="str">
         <x:f t="shared" si="2"/>
@@ -2492,34 +2412,24 @@
       <x:c r="B52" s="9">
         <x:v>28</x:v>
       </x:c>
-      <x:c r="C52" s="35" t="n">
-        <x:v>MOTOR RAUL DIAZ PALACIOS</x:v>
-      </x:c>
+      <x:c r="C52" s="35"/>
       <x:c r="D52" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="E52" s="36" t="n">
-        <x:v>18174774</x:v>
-      </x:c>
-      <x:c r="F52" s="35" t="n">
-        <x:v>000674725663</x:v>
-      </x:c>
-      <x:c r="G52" s="40" t="n">
+      <x:c r="E52" s="36"/>
+      <x:c r="F52" s="35"/>
+      <x:c r="G52" s="40" t="str">
         <x:f t="shared" si="0"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="H52" s="35" t="n">
-        <x:v>364.22</x:v>
-      </x:c>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="H52" s="35"/>
       <x:c r="I52" s="40" t="n">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="J52" s="42" t="n">
-        <x:v>13,472.99</x:v>
-      </x:c>
-      <x:c r="K52" s="43" t="n">
-        <x:v>SOL</x:v>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="J52" s="42"/>
+      <x:c r="K52" s="43" t="s">
+        <x:v>37</x:v>
       </x:c>
       <x:c r="M52" s="22" t="str">
         <x:f t="shared" si="2"/>
@@ -2530,34 +2440,24 @@
       <x:c r="B53" s="9">
         <x:v>29</x:v>
       </x:c>
-      <x:c r="C53" s="35" t="n">
-        <x:v>MIRO IVAN SILVA MOLINA</x:v>
-      </x:c>
+      <x:c r="C53" s="35"/>
       <x:c r="D53" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="E53" s="36" t="n">
-        <x:v>32956376</x:v>
-      </x:c>
-      <x:c r="F53" s="35" t="n">
-        <x:v>000586680330</x:v>
-      </x:c>
-      <x:c r="G53" s="40" t="n">
+      <x:c r="E53" s="36"/>
+      <x:c r="F53" s="35"/>
+      <x:c r="G53" s="40" t="str">
         <x:f t="shared" si="0"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="H53" s="35" t="n">
-        <x:v>333.31</x:v>
-      </x:c>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="H53" s="35"/>
       <x:c r="I53" s="40" t="n">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="J53" s="42" t="n">
-        <x:v>5,405.16</x:v>
-      </x:c>
-      <x:c r="K53" s="43" t="n">
-        <x:v>SOL</x:v>
+        <x:v>'SOL</x:v>
+      </x:c>
+      <x:c r="J53" s="42"/>
+      <x:c r="K53" s="43" t="s">
+        <x:v>37</x:v>
       </x:c>
       <x:c r="M53" s="22" t="str">
         <x:f t="shared" si="2"/>
@@ -2568,34 +2468,24 @@
       <x:c r="B54" s="9">
         <x:v>30</x:v>
       </x:c>
-      <x:c r="C54" s="35" t="n">
-        <x:v>BLADIMIRO ESTRADA MENDIETA</x:v>
-      </x:c>
+      <x:c r="C54" s="35"/>
       <x:c r="D54" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="E54" s="36" t="n">
-        <x:v>32950996</x:v>
-      </x:c>
-      <x:c r="F54" s="35" t="n">
-        <x:v>000606643745</x:v>
-      </x:c>
-      <x:c r="G54" s="40" t="n">
+      <x:c r="E54" s="36"/>
+      <x:c r="F54" s="35"/>
+      <x:c r="G54" s="40" t="str">
         <x:f t="shared" si="0"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="H54" s="35" t="n">
-        <x:v>187.03</x:v>
-      </x:c>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="H54" s="35"/>
       <x:c r="I54" s="40" t="n">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="J54" s="42" t="n">
-        <x:v>21,849.73</x:v>
-      </x:c>
-      <x:c r="K54" s="43" t="n">
-        <x:v>SOL</x:v>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="J54" s="42"/>
+      <x:c r="K54" s="43" t="s">
+        <x:v>37</x:v>
       </x:c>
       <x:c r="M54" s="22" t="str">
         <x:f t="shared" si="2"/>
@@ -2606,34 +2496,24 @@
       <x:c r="B55" s="9">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="C55" s="35" t="n">
-        <x:v>WALTER CELESTINO CHAVEZ RODRIGUEZ</x:v>
-      </x:c>
+      <x:c r="C55" s="35"/>
       <x:c r="D55" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="E55" s="36" t="n">
-        <x:v>15852525</x:v>
-      </x:c>
-      <x:c r="F55" s="35" t="n">
-        <x:v>000622560264</x:v>
-      </x:c>
-      <x:c r="G55" s="40" t="n">
+      <x:c r="E55" s="36"/>
+      <x:c r="F55" s="35"/>
+      <x:c r="G55" s="40" t="str">
         <x:f t="shared" si="0"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="H55" s="35" t="n">
-        <x:v>304.05</x:v>
-      </x:c>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="H55" s="35"/>
       <x:c r="I55" s="40" t="n">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="J55" s="42" t="n">
-        <x:v>24,974.30</x:v>
-      </x:c>
-      <x:c r="K55" s="43" t="n">
-        <x:v>SOL</x:v>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="J55" s="42"/>
+      <x:c r="K55" s="43" t="s">
+        <x:v>37</x:v>
       </x:c>
       <x:c r="M55" s="22" t="str">
         <x:f t="shared" si="2"/>
@@ -2644,34 +2524,24 @@
       <x:c r="B56" s="9">
         <x:v>32</x:v>
       </x:c>
-      <x:c r="C56" s="35" t="n">
-        <x:v>EDWIN ORESTES MEJIA LUNA</x:v>
-      </x:c>
+      <x:c r="C56" s="35"/>
       <x:c r="D56" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="E56" s="36" t="n">
-        <x:v>15712932</x:v>
-      </x:c>
-      <x:c r="F56" s="35" t="n">
-        <x:v>000622579990</x:v>
-      </x:c>
-      <x:c r="G56" s="40" t="n">
+      <x:c r="E56" s="36"/>
+      <x:c r="F56" s="35"/>
+      <x:c r="G56" s="40" t="str">
         <x:f t="shared" si="0"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="H56" s="35" t="n">
-        <x:v>178.47</x:v>
-      </x:c>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="H56" s="35"/>
       <x:c r="I56" s="40" t="n">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="J56" s="42" t="n">
-        <x:v>26,302.59</x:v>
-      </x:c>
-      <x:c r="K56" s="43" t="n">
-        <x:v>SOL</x:v>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="J56" s="42"/>
+      <x:c r="K56" s="43" t="s">
+        <x:v>37</x:v>
       </x:c>
       <x:c r="M56" s="22" t="str">
         <x:f t="shared" si="2"/>
@@ -2682,34 +2552,24 @@
       <x:c r="B57" s="9">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="C57" s="35" t="n">
-        <x:v>SANTOS AUGUSTO MEJIA LUNA</x:v>
-      </x:c>
+      <x:c r="C57" s="35"/>
       <x:c r="D57" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="E57" s="36" t="n">
-        <x:v>32892888</x:v>
-      </x:c>
-      <x:c r="F57" s="35" t="n">
-        <x:v>000674937820</x:v>
-      </x:c>
-      <x:c r="G57" s="40" t="n">
+      <x:c r="E57" s="36"/>
+      <x:c r="F57" s="35"/>
+      <x:c r="G57" s="40" t="str">
         <x:f t="shared" si="0"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="H57" s="35" t="n">
-        <x:v>390.62</x:v>
-      </x:c>
-      <x:c r="I57" s="40" t="n">
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="H57" s="35"/>
+      <x:c r="I57" s="40" t="str">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="J57" s="42" t="n">
-        <x:v>14,947.61</x:v>
-      </x:c>
-      <x:c r="K57" s="43" t="n">
-        <x:v>SOL</x:v>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="J57" s="42"/>
+      <x:c r="K57" s="43" t="s">
+        <x:v>37</x:v>
       </x:c>
       <x:c r="M57" s="22" t="str">
         <x:f t="shared" si="2"/>
@@ -2720,34 +2580,24 @@
       <x:c r="B58" s="9">
         <x:v>34</x:v>
       </x:c>
-      <x:c r="C58" s="35" t="n">
-        <x:v>LUIS GONZALES CAMPOS</x:v>
-      </x:c>
+      <x:c r="C58" s="35"/>
       <x:c r="D58" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="E58" s="36" t="n">
-        <x:v>32734045</x:v>
-      </x:c>
-      <x:c r="F58" s="35" t="n">
-        <x:v>000624141920</x:v>
-      </x:c>
-      <x:c r="G58" s="40" t="n">
+      <x:c r="E58" s="36"/>
+      <x:c r="F58" s="35"/>
+      <x:c r="G58" s="40" t="str">
         <x:f t="shared" si="0"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="H58" s="35" t="n">
-        <x:v>307.73</x:v>
-      </x:c>
-      <x:c r="I58" s="40" t="n">
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="H58" s="35"/>
+      <x:c r="I58" s="40" t="str">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="J58" s="42" t="n">
-        <x:v>2,098.70</x:v>
-      </x:c>
-      <x:c r="K58" s="43" t="n">
-        <x:v>SOL</x:v>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="J58" s="42"/>
+      <x:c r="K58" s="43" t="s">
+        <x:v>37</x:v>
       </x:c>
       <x:c r="M58" s="22" t="str">
         <x:f t="shared" si="2"/>
@@ -2758,34 +2608,24 @@
       <x:c r="B59" s="9">
         <x:v>35</x:v>
       </x:c>
-      <x:c r="C59" s="35" t="n">
-        <x:v>JOSE FERNANDO HORNA OORREA</x:v>
-      </x:c>
+      <x:c r="C59" s="35"/>
       <x:c r="D59" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="E59" s="36" t="n">
-        <x:v>16023843</x:v>
-      </x:c>
-      <x:c r="F59" s="35" t="n">
-        <x:v>000669449954</x:v>
-      </x:c>
-      <x:c r="G59" s="40" t="n">
+      <x:c r="E59" s="36"/>
+      <x:c r="F59" s="35"/>
+      <x:c r="G59" s="40" t="str">
         <x:f t="shared" si="0"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="H59" s="35" t="n">
-        <x:v>238.52</x:v>
-      </x:c>
-      <x:c r="I59" s="40" t="n">
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="H59" s="35"/>
+      <x:c r="I59" s="40" t="str">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="J59" s="42" t="n">
-        <x:v>5,775.88</x:v>
-      </x:c>
-      <x:c r="K59" s="43" t="n">
-        <x:v>SOL</x:v>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="J59" s="42"/>
+      <x:c r="K59" s="43" t="s">
+        <x:v>37</x:v>
       </x:c>
       <x:c r="M59" s="22" t="str">
         <x:f t="shared" si="2"/>
@@ -2796,34 +2636,24 @@
       <x:c r="B60" s="9">
         <x:v>36</x:v>
       </x:c>
-      <x:c r="C60" s="35" t="n">
-        <x:v>ALEJANDRO VALENTIN MORA GAMBOA</x:v>
-      </x:c>
+      <x:c r="C60" s="35"/>
       <x:c r="D60" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="E60" s="36" t="n">
-        <x:v>32937828</x:v>
-      </x:c>
-      <x:c r="F60" s="35" t="n">
-        <x:v>000596062134</x:v>
-      </x:c>
-      <x:c r="G60" s="40" t="n">
+      <x:c r="E60" s="36"/>
+      <x:c r="F60" s="35"/>
+      <x:c r="G60" s="40" t="str">
         <x:f t="shared" si="0"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="H60" s="35" t="n">
-        <x:v>191.23</x:v>
-      </x:c>
-      <x:c r="I60" s="40" t="n">
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="H60" s="35"/>
+      <x:c r="I60" s="40" t="str">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="J60" s="42" t="n">
-        <x:v>11,604.05</x:v>
-      </x:c>
-      <x:c r="K60" s="43" t="n">
-        <x:v>SOL</x:v>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="J60" s="42"/>
+      <x:c r="K60" s="43" t="s">
+        <x:v>37</x:v>
       </x:c>
       <x:c r="M60" s="22" t="str">
         <x:f t="shared" si="2"/>
@@ -2834,34 +2664,24 @@
       <x:c r="B61" s="9">
         <x:v>37</x:v>
       </x:c>
-      <x:c r="C61" s="35" t="n">
-        <x:v>MARCELINO SEVILLANO OLORTIGUE</x:v>
-      </x:c>
+      <x:c r="C61" s="35"/>
       <x:c r="D61" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="E61" s="36" t="n">
-        <x:v>32863288</x:v>
-      </x:c>
-      <x:c r="F61" s="35" t="n">
-        <x:v>000582046688</x:v>
-      </x:c>
-      <x:c r="G61" s="40" t="n">
+      <x:c r="E61" s="36"/>
+      <x:c r="F61" s="35"/>
+      <x:c r="G61" s="40" t="str">
         <x:f t="shared" si="0"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="H61" s="35" t="n">
-        <x:v>118.86</x:v>
-      </x:c>
-      <x:c r="I61" s="40" t="n">
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="H61" s="35"/>
+      <x:c r="I61" s="40" t="str">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="J61" s="42" t="n">
-        <x:v>2,320.00</x:v>
-      </x:c>
-      <x:c r="K61" s="43" t="n">
-        <x:v>SOL</x:v>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="J61" s="42"/>
+      <x:c r="K61" s="43" t="s">
+        <x:v>37</x:v>
       </x:c>
       <x:c r="M61" s="22" t="str">
         <x:f t="shared" si="2"/>
@@ -2872,34 +2692,24 @@
       <x:c r="B62" s="9">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="C62" s="35" t="n">
-        <x:v>WILFREDO DIDI MARINOS PEREDA</x:v>
-      </x:c>
+      <x:c r="C62" s="35"/>
       <x:c r="D62" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="E62" s="36" t="n">
-        <x:v>32908422</x:v>
-      </x:c>
-      <x:c r="F62" s="35" t="n">
-        <x:v>000679932623</x:v>
-      </x:c>
-      <x:c r="G62" s="40" t="n">
+      <x:c r="E62" s="36"/>
+      <x:c r="F62" s="35"/>
+      <x:c r="G62" s="40" t="str">
         <x:f t="shared" si="0"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="H62" s="35" t="n">
-        <x:v>318.29</x:v>
-      </x:c>
-      <x:c r="I62" s="40" t="n">
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="H62" s="35"/>
+      <x:c r="I62" s="40" t="str">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="J62" s="42" t="n">
-        <x:v>17,778.43</x:v>
-      </x:c>
-      <x:c r="K62" s="43" t="n">
-        <x:v>SOL</x:v>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="J62" s="42"/>
+      <x:c r="K62" s="43" t="s">
+        <x:v>37</x:v>
       </x:c>
       <x:c r="M62" s="22" t="str">
         <x:f t="shared" si="2"/>
@@ -2910,34 +2720,24 @@
       <x:c r="B63" s="9">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="C63" s="35" t="n">
-        <x:v>WALTER GENARO NATIVIDAD SANDONAS</x:v>
-      </x:c>
+      <x:c r="C63" s="35"/>
       <x:c r="D63" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="E63" s="36" t="n">
-        <x:v>32906767</x:v>
-      </x:c>
-      <x:c r="F63" s="35" t="n">
-        <x:v>000943135893</x:v>
-      </x:c>
-      <x:c r="G63" s="40" t="n">
+      <x:c r="E63" s="36"/>
+      <x:c r="F63" s="35"/>
+      <x:c r="G63" s="40" t="str">
         <x:f t="shared" si="0"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="H63" s="35" t="n">
-        <x:v>327.45</x:v>
-      </x:c>
-      <x:c r="I63" s="40" t="n">
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="H63" s="35"/>
+      <x:c r="I63" s="40" t="str">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="J63" s="42" t="n">
-        <x:v>33.44521</x:v>
-      </x:c>
-      <x:c r="K63" s="43" t="n">
-        <x:v>SOL</x:v>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="J63" s="42"/>
+      <x:c r="K63" s="43" t="s">
+        <x:v>37</x:v>
       </x:c>
       <x:c r="M63" s="22" t="str">
         <x:f t="shared" si="2"/>
@@ -2948,34 +2748,24 @@
       <x:c r="B64" s="9">
         <x:v>40</x:v>
       </x:c>
-      <x:c r="C64" s="35" t="n">
-        <x:v>SEGUNDO PEDRO CUEVA HUARAZ</x:v>
-      </x:c>
+      <x:c r="C64" s="35"/>
       <x:c r="D64" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="E64" s="36" t="n">
-        <x:v>32116960</x:v>
-      </x:c>
-      <x:c r="F64" s="35" t="n">
-        <x:v>000669589268</x:v>
-      </x:c>
-      <x:c r="G64" s="40" t="n">
+      <x:c r="E64" s="36"/>
+      <x:c r="F64" s="35"/>
+      <x:c r="G64" s="40" t="str">
         <x:f t="shared" si="0"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="H64" s="35" t="n">
-        <x:v>327.45</x:v>
-      </x:c>
-      <x:c r="I64" s="40" t="n">
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="H64" s="35"/>
+      <x:c r="I64" s="40" t="str">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="J64" s="42" t="n">
-        <x:v>31,996.00</x:v>
-      </x:c>
-      <x:c r="K64" s="43" t="n">
-        <x:v>SOL</x:v>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="J64" s="42"/>
+      <x:c r="K64" s="43" t="s">
+        <x:v>37</x:v>
       </x:c>
       <x:c r="M64" s="22" t="str">
         <x:f t="shared" si="2"/>
@@ -2986,34 +2776,24 @@
       <x:c r="B65" s="9">
         <x:v>41</x:v>
       </x:c>
-      <x:c r="C65" s="35" t="n">
-        <x:v>RAUL VALENTIN GULARTE MALDONADO</x:v>
-      </x:c>
+      <x:c r="C65" s="35"/>
       <x:c r="D65" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="E65" s="36" t="n">
-        <x:v>41122711</x:v>
-      </x:c>
-      <x:c r="F65" s="35" t="n">
-        <x:v>000665645000</x:v>
-      </x:c>
-      <x:c r="G65" s="40" t="n">
+      <x:c r="E65" s="36"/>
+      <x:c r="F65" s="35"/>
+      <x:c r="G65" s="40" t="str">
         <x:f t="shared" si="0"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="H65" s="35" t="n">
-        <x:v>129.48</x:v>
-      </x:c>
-      <x:c r="I65" s="40" t="n">
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="H65" s="35"/>
+      <x:c r="I65" s="40" t="str">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="J65" s="42" t="n">
-        <x:v>35,617.54</x:v>
-      </x:c>
-      <x:c r="K65" s="43" t="n">
-        <x:v>SOL</x:v>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="J65" s="42"/>
+      <x:c r="K65" s="43" t="s">
+        <x:v>37</x:v>
       </x:c>
       <x:c r="M65" s="22" t="str">
         <x:f t="shared" si="2"/>
@@ -3024,34 +2804,24 @@
       <x:c r="B66" s="9">
         <x:v>42</x:v>
       </x:c>
-      <x:c r="C66" s="35" t="n">
-        <x:v>LUIS LENNY SANTILLAN ORTIZ</x:v>
-      </x:c>
+      <x:c r="C66" s="35"/>
       <x:c r="D66" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="E66" s="36" t="n">
-        <x:v>32978938</x:v>
-      </x:c>
-      <x:c r="F66" s="35" t="n">
-        <x:v>000606459774</x:v>
-      </x:c>
-      <x:c r="G66" s="40" t="n">
+      <x:c r="E66" s="36"/>
+      <x:c r="F66" s="35"/>
+      <x:c r="G66" s="40" t="str">
         <x:f t="shared" si="0"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="H66" s="35" t="n">
-        <x:v>1,135.62</x:v>
-      </x:c>
-      <x:c r="I66" s="40" t="n">
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="H66" s="35"/>
+      <x:c r="I66" s="40" t="str">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="J66" s="42" t="n">
-        <x:v>2,400.00</x:v>
-      </x:c>
-      <x:c r="K66" s="43" t="n">
-        <x:v>SOL</x:v>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="J66" s="42"/>
+      <x:c r="K66" s="43" t="s">
+        <x:v>37</x:v>
       </x:c>
       <x:c r="M66" s="22" t="str">
         <x:f t="shared" si="2"/>
@@ -3062,34 +2832,24 @@
       <x:c r="B67" s="9">
         <x:v>43</x:v>
       </x:c>
-      <x:c r="C67" s="35" t="n">
-        <x:v>JORGEJUAN FLORES CASTILLO</x:v>
-      </x:c>
+      <x:c r="C67" s="35"/>
       <x:c r="D67" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="E67" s="36" t="n">
-        <x:v>15977502</x:v>
-      </x:c>
-      <x:c r="F67" s="35" t="n">
-        <x:v>000669449903</x:v>
-      </x:c>
-      <x:c r="G67" s="40" t="n">
+      <x:c r="E67" s="36"/>
+      <x:c r="F67" s="35"/>
+      <x:c r="G67" s="40" t="str">
         <x:f t="shared" si="0"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="H67" s="35" t="n">
-        <x:v>203.63</x:v>
-      </x:c>
-      <x:c r="I67" s="40" t="n">
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="H67" s="35"/>
+      <x:c r="I67" s="40" t="str">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="J67" s="42" t="n">
-        <x:v>3,093.99</x:v>
-      </x:c>
-      <x:c r="K67" s="43" t="n">
-        <x:v>SOL</x:v>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="J67" s="42"/>
+      <x:c r="K67" s="43" t="s">
+        <x:v>37</x:v>
       </x:c>
       <x:c r="M67" s="22" t="str">
         <x:f t="shared" si="2"/>
@@ -3100,34 +2860,24 @@
       <x:c r="B68" s="9">
         <x:v>44</x:v>
       </x:c>
-      <x:c r="C68" s="35" t="n">
-        <x:v>YSMAEL HIDALGO FIGUEROA REYNA</x:v>
-      </x:c>
+      <x:c r="C68" s="35"/>
       <x:c r="D68" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="E68" s="36" t="n">
-        <x:v>32875603</x:v>
-      </x:c>
-      <x:c r="F68" s="35" t="n">
-        <x:v>000554677309</x:v>
-      </x:c>
-      <x:c r="G68" s="40" t="n">
+      <x:c r="E68" s="36"/>
+      <x:c r="F68" s="35"/>
+      <x:c r="G68" s="40" t="str">
         <x:f t="shared" si="0"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="H68" s="35" t="n">
-        <x:v>214.17</x:v>
-      </x:c>
-      <x:c r="I68" s="40" t="n">
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="H68" s="35"/>
+      <x:c r="I68" s="40" t="str">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="J68" s="42" t="n">
-        <x:v>7,936.23</x:v>
-      </x:c>
-      <x:c r="K68" s="43" t="n">
-        <x:v>SOL</x:v>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="J68" s="42"/>
+      <x:c r="K68" s="43" t="s">
+        <x:v>37</x:v>
       </x:c>
       <x:c r="M68" s="22" t="str">
         <x:f t="shared" si="2"/>
@@ -3138,34 +2888,24 @@
       <x:c r="B69" s="9">
         <x:v>45</x:v>
       </x:c>
-      <x:c r="C69" s="35" t="n">
-        <x:v>EDUARDO NORIEGA CARBAJAL</x:v>
-      </x:c>
+      <x:c r="C69" s="35"/>
       <x:c r="D69" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="E69" s="36" t="n">
-        <x:v>40668907</x:v>
-      </x:c>
-      <x:c r="F69" s="35" t="n">
-        <x:v>000964424593</x:v>
-      </x:c>
-      <x:c r="G69" s="40" t="n">
+      <x:c r="E69" s="36"/>
+      <x:c r="F69" s="35"/>
+      <x:c r="G69" s="40" t="str">
         <x:f t="shared" si="0"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="H69" s="35" t="n">
-        <x:v>307.73</x:v>
-      </x:c>
-      <x:c r="I69" s="40" t="n">
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="H69" s="35"/>
+      <x:c r="I69" s="40" t="str">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="J69" s="42" t="n">
-        <x:v>23,109.60</x:v>
-      </x:c>
-      <x:c r="K69" s="43" t="n">
-        <x:v>SOL</x:v>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="J69" s="42"/>
+      <x:c r="K69" s="43" t="s">
+        <x:v>37</x:v>
       </x:c>
       <x:c r="M69" s="22" t="str">
         <x:f t="shared" si="2"/>
@@ -3176,34 +2916,24 @@
       <x:c r="B70" s="9">
         <x:v>46</x:v>
       </x:c>
-      <x:c r="C70" s="35" t="n">
-        <x:v>HENRY ALEXANDER RAMIREZ FLORES</x:v>
-      </x:c>
+      <x:c r="C70" s="35"/>
       <x:c r="D70" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="E70" s="36" t="n">
-        <x:v>32963500</x:v>
-      </x:c>
-      <x:c r="F70" s="35" t="n">
-        <x:v>000797560490</x:v>
-      </x:c>
-      <x:c r="G70" s="40" t="n">
+      <x:c r="E70" s="36"/>
+      <x:c r="F70" s="35"/>
+      <x:c r="G70" s="40" t="str">
         <x:f t="shared" si="0"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="H70" s="35" t="n">
-        <x:v>434.58</x:v>
-      </x:c>
-      <x:c r="I70" s="40" t="n">
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="H70" s="35"/>
+      <x:c r="I70" s="40" t="str">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="J70" s="42" t="n">
-        <x:v>3,166.70</x:v>
-      </x:c>
-      <x:c r="K70" s="43" t="n">
-        <x:v>SOL</x:v>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="J70" s="42"/>
+      <x:c r="K70" s="43" t="s">
+        <x:v>37</x:v>
       </x:c>
       <x:c r="M70" s="22" t="str">
         <x:f t="shared" si="2"/>
@@ -3214,34 +2944,24 @@
       <x:c r="B71" s="9">
         <x:v>47</x:v>
       </x:c>
-      <x:c r="C71" s="35" t="n">
-        <x:v>HIMBERTH JOSE TIRADO OLAZABAL</x:v>
-      </x:c>
+      <x:c r="C71" s="35"/>
       <x:c r="D71" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="E71" s="36" t="n">
-        <x:v>32937979</x:v>
-      </x:c>
-      <x:c r="F71" s="35" t="n">
-        <x:v>000596065176</x:v>
-      </x:c>
-      <x:c r="G71" s="40" t="n">
+      <x:c r="E71" s="36"/>
+      <x:c r="F71" s="35"/>
+      <x:c r="G71" s="40" t="str">
         <x:f t="shared" si="0"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="H71" s="35" t="n">
-        <x:v>173.76</x:v>
-      </x:c>
-      <x:c r="I71" s="40" t="n">
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="H71" s="35"/>
+      <x:c r="I71" s="40" t="str">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="J71" s="42" t="n">
-        <x:v>5,641.09</x:v>
-      </x:c>
-      <x:c r="K71" s="43" t="n">
-        <x:v>SOL</x:v>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="J71" s="42"/>
+      <x:c r="K71" s="43" t="s">
+        <x:v>37</x:v>
       </x:c>
       <x:c r="M71" s="22" t="str">
         <x:f t="shared" si="2"/>
@@ -3252,34 +2972,24 @@
       <x:c r="B72" s="9">
         <x:v>48</x:v>
       </x:c>
-      <x:c r="C72" s="35" t="n">
-        <x:v>PEDRO GABRIEL MENDOZA LEON</x:v>
-      </x:c>
+      <x:c r="C72" s="35"/>
       <x:c r="D72" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="E72" s="36" t="n">
-        <x:v>41394454</x:v>
-      </x:c>
-      <x:c r="F72" s="35" t="n">
-        <x:v>000624050207</x:v>
-      </x:c>
-      <x:c r="G72" s="40" t="n">
+      <x:c r="E72" s="36"/>
+      <x:c r="F72" s="35"/>
+      <x:c r="G72" s="40" t="str">
         <x:f t="shared" si="0"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="H72" s="35" t="n">
-        <x:v>99.57</x:v>
-      </x:c>
-      <x:c r="I72" s="40" t="n">
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="H72" s="35"/>
+      <x:c r="I72" s="40" t="str">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="J72" s="42" t="n">
-        <x:v>12,693.79</x:v>
-      </x:c>
-      <x:c r="K72" s="43" t="n">
-        <x:v>SOL</x:v>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="J72" s="42"/>
+      <x:c r="K72" s="43" t="s">
+        <x:v>37</x:v>
       </x:c>
       <x:c r="M72" s="22" t="str">
         <x:f t="shared" si="2"/>
@@ -3290,34 +3000,24 @@
       <x:c r="B73" s="9">
         <x:v>49</x:v>
       </x:c>
-      <x:c r="C73" s="35" t="n">
-        <x:v>HUMBERTO VILLACORTA LUNA</x:v>
-      </x:c>
+      <x:c r="C73" s="35"/>
       <x:c r="D73" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="E73" s="36" t="n">
-        <x:v>32990883</x:v>
-      </x:c>
-      <x:c r="F73" s="35" t="n">
-        <x:v>000566265704</x:v>
-      </x:c>
-      <x:c r="G73" s="40" t="n">
+      <x:c r="E73" s="36"/>
+      <x:c r="F73" s="35"/>
+      <x:c r="G73" s="40" t="str">
         <x:f t="shared" si="0"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="H73" s="35" t="n">
-        <x:v>230.95</x:v>
-      </x:c>
-      <x:c r="I73" s="40" t="n">
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="H73" s="35"/>
+      <x:c r="I73" s="40" t="str">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="J73" s="42" t="n">
-        <x:v>7,286.97</x:v>
-      </x:c>
-      <x:c r="K73" s="43" t="n">
-        <x:v>SOL</x:v>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="J73" s="42"/>
+      <x:c r="K73" s="43" t="s">
+        <x:v>37</x:v>
       </x:c>
       <x:c r="M73" s="22" t="str">
         <x:f t="shared" si="2"/>
@@ -3328,34 +3028,24 @@
       <x:c r="B74" s="9">
         <x:v>50</x:v>
       </x:c>
-      <x:c r="C74" s="35" t="n">
-        <x:v>WILLIAM ANTENOR MARCELO CASAHUAMAN</x:v>
-      </x:c>
+      <x:c r="C74" s="35"/>
       <x:c r="D74" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="E74" s="36" t="n">
-        <x:v>25831929</x:v>
-      </x:c>
-      <x:c r="F74" s="35" t="n">
-        <x:v>000596676666</x:v>
-      </x:c>
+      <x:c r="E74" s="36"/>
+      <x:c r="F74" s="35"/>
       <x:c r="G74" s="40" t="str">
         <x:f t="shared" si="0"/>
         <x:v>SOL</x:v>
       </x:c>
-      <x:c r="H74" s="35" t="n">
-        <x:v>336.51</x:v>
-      </x:c>
-      <x:c r="I74" s="40" t="n">
+      <x:c r="H74" s="35"/>
+      <x:c r="I74" s="40" t="str">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="J74" s="42" t="n">
-        <x:v>2,895.85</x:v>
-      </x:c>
-      <x:c r="K74" s="43" t="n">
-        <x:v>SOL</x:v>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="J74" s="42"/>
+      <x:c r="K74" s="43" t="s">
+        <x:v>37</x:v>
       </x:c>
       <x:c r="M74" s="22" t="str">
         <x:f t="shared" si="2"/>
@@ -3366,34 +3056,24 @@
       <x:c r="B75" s="9">
         <x:v>51</x:v>
       </x:c>
-      <x:c r="C75" s="35" t="n">
-        <x:v>JOSE WILMER FIESTAS PURIZACA</x:v>
-      </x:c>
+      <x:c r="C75" s="35"/>
       <x:c r="D75" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="E75" s="36" t="n">
-        <x:v>02799578</x:v>
-      </x:c>
-      <x:c r="F75" s="35" t="n">
-        <x:v>000685835855</x:v>
-      </x:c>
+      <x:c r="E75" s="36"/>
+      <x:c r="F75" s="35"/>
       <x:c r="G75" s="40" t="str">
         <x:f t="shared" si="0"/>
         <x:v>SOL</x:v>
       </x:c>
-      <x:c r="H75" s="35" t="n">
-        <x:v>525.47</x:v>
-      </x:c>
-      <x:c r="I75" s="40" t="n">
+      <x:c r="H75" s="35"/>
+      <x:c r="I75" s="40" t="str">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="J75" s="42" t="n">
-        <x:v>9,091.84</x:v>
-      </x:c>
-      <x:c r="K75" s="43" t="n">
-        <x:v>SOL</x:v>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="J75" s="42"/>
+      <x:c r="K75" s="43" t="s">
+        <x:v>37</x:v>
       </x:c>
       <x:c r="M75" s="22" t="str">
         <x:f t="shared" si="2"/>
@@ -3404,32 +3084,24 @@
       <x:c r="B76" s="9">
         <x:v>52</x:v>
       </x:c>
-      <x:c r="C76" s="35" t="n">
-        <x:v>CESAR AUGUSTO GARCIA GUAYLUPO</x:v>
-      </x:c>
+      <x:c r="C76" s="35"/>
       <x:c r="D76" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="E76" s="36" t="n">
-        <x:v>09824142</x:v>
-      </x:c>
-      <x:c r="F76" s="35" t="n">
-        <x:v>000573134375</x:v>
-      </x:c>
+      <x:c r="E76" s="36"/>
+      <x:c r="F76" s="35"/>
       <x:c r="G76" s="40" t="str">
         <x:f t="shared" si="0"/>
         <x:v>SOL</x:v>
       </x:c>
       <x:c r="H76" s="35"/>
-      <x:c r="I76" s="40" t="n">
+      <x:c r="I76" s="40" t="str">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
-      </x:c>
-      <x:c r="J76" s="42" t="n">
-        <x:v>23,937.59</x:v>
-      </x:c>
-      <x:c r="K76" s="43" t="n">
-        <x:v>SOL</x:v>
+        <x:v>SOL</x:v>
+      </x:c>
+      <x:c r="J76" s="42"/>
+      <x:c r="K76" s="43" t="s">
+        <x:v>37</x:v>
       </x:c>
       <x:c r="M76" s="22" t="str">
         <x:f t="shared" si="2"/>
@@ -3440,9 +3112,7 @@
       <x:c r="B77" s="9">
         <x:v>53</x:v>
       </x:c>
-      <x:c r="C77" s="35" t="n">
-        <x:v>JOSE MIGUEL RIVERA RUBIO</x:v>
-      </x:c>
+      <x:c r="C77" s="35"/>
       <x:c r="D77" s="32" t="s">
         <x:v>38</x:v>
       </x:c>
@@ -3453,9 +3123,9 @@
         <x:v>SOL</x:v>
       </x:c>
       <x:c r="H77" s="35"/>
-      <x:c r="I77" s="40" t="n">
+      <x:c r="I77" s="40" t="str">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
+        <x:v>SOL</x:v>
       </x:c>
       <x:c r="J77" s="42"/>
       <x:c r="K77" s="43" t="s">
@@ -3481,9 +3151,9 @@
         <x:v>SOL</x:v>
       </x:c>
       <x:c r="H78" s="35"/>
-      <x:c r="I78" s="40" t="n">
+      <x:c r="I78" s="40" t="str">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
+        <x:v>SOL</x:v>
       </x:c>
       <x:c r="J78" s="42"/>
       <x:c r="K78" s="43" t="s">
@@ -3509,9 +3179,9 @@
         <x:v>SOL</x:v>
       </x:c>
       <x:c r="H79" s="35"/>
-      <x:c r="I79" s="40" t="n">
+      <x:c r="I79" s="40" t="str">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
+        <x:v>SOL</x:v>
       </x:c>
       <x:c r="J79" s="42"/>
       <x:c r="K79" s="43" t="s">
@@ -3535,9 +3205,9 @@
         <x:v>SOL</x:v>
       </x:c>
       <x:c r="H80" s="35"/>
-      <x:c r="I80" s="40" t="n">
+      <x:c r="I80" s="40" t="str">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
+        <x:v>SOL</x:v>
       </x:c>
       <x:c r="J80" s="42"/>
       <x:c r="K80" s="43"/>
@@ -3559,9 +3229,9 @@
         <x:v>SOL</x:v>
       </x:c>
       <x:c r="H81" s="35"/>
-      <x:c r="I81" s="40" t="n">
+      <x:c r="I81" s="40" t="str">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
+        <x:v>SOL</x:v>
       </x:c>
       <x:c r="J81" s="42"/>
       <x:c r="K81" s="43"/>
@@ -3583,9 +3253,9 @@
         <x:v>SOL</x:v>
       </x:c>
       <x:c r="H82" s="35"/>
-      <x:c r="I82" s="40" t="n">
+      <x:c r="I82" s="40" t="str">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
+        <x:v>SOL</x:v>
       </x:c>
       <x:c r="J82" s="42"/>
       <x:c r="K82" s="43"/>
@@ -3607,9 +3277,9 @@
         <x:v>SOL</x:v>
       </x:c>
       <x:c r="H83" s="35"/>
-      <x:c r="I83" s="40" t="n">
+      <x:c r="I83" s="40" t="str">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
+        <x:v>SOL</x:v>
       </x:c>
       <x:c r="J83" s="42"/>
       <x:c r="K83" s="43"/>
@@ -3631,9 +3301,9 @@
         <x:v>SOL</x:v>
       </x:c>
       <x:c r="H84" s="35"/>
-      <x:c r="I84" s="40" t="n">
+      <x:c r="I84" s="40" t="str">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
+        <x:v>SOL</x:v>
       </x:c>
       <x:c r="J84" s="42"/>
       <x:c r="K84" s="43"/>
@@ -3655,9 +3325,9 @@
         <x:v>SOL</x:v>
       </x:c>
       <x:c r="H85" s="35"/>
-      <x:c r="I85" s="40" t="n">
+      <x:c r="I85" s="40" t="str">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
+        <x:v>SOL</x:v>
       </x:c>
       <x:c r="J85" s="42"/>
       <x:c r="K85" s="43"/>
@@ -3679,9 +3349,9 @@
         <x:v>SOL</x:v>
       </x:c>
       <x:c r="H86" s="35"/>
-      <x:c r="I86" s="40" t="n">
+      <x:c r="I86" s="40" t="str">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
+        <x:v>SOL</x:v>
       </x:c>
       <x:c r="J86" s="35"/>
       <x:c r="K86" s="43"/>
@@ -3703,9 +3373,9 @@
         <x:v>SOL</x:v>
       </x:c>
       <x:c r="H87" s="35"/>
-      <x:c r="I87" s="40" t="n">
+      <x:c r="I87" s="40" t="str">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
+        <x:v>SOL</x:v>
       </x:c>
       <x:c r="J87" s="35"/>
       <x:c r="K87" s="43"/>
@@ -3727,9 +3397,9 @@
         <x:v>SOL</x:v>
       </x:c>
       <x:c r="H88" s="35"/>
-      <x:c r="I88" s="40" t="n">
+      <x:c r="I88" s="40" t="str">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
+        <x:v>SOL</x:v>
       </x:c>
       <x:c r="J88" s="35"/>
       <x:c r="K88" s="43"/>
@@ -3751,9 +3421,9 @@
         <x:v>SOL</x:v>
       </x:c>
       <x:c r="H89" s="35"/>
-      <x:c r="I89" s="40" t="n">
+      <x:c r="I89" s="40" t="str">
         <x:f t="shared" si="1"/>
-        <x:v>DOL</x:v>
+        <x:v>SOL</x:v>
       </x:c>
       <x:c r="J89" s="35"/>
       <x:c r="K89" s="43"/>
@@ -3775,9 +3445,9 @@
         <x:v>SOL</x:v>
       </x:c>
       <x:c r="H90" s="35"/>
-      <x:c r="I90" s="40" t="n">
+      <x:c r="I90" s="40" t="str">
         <x:f t="shared" ref="I90:I153" si="4">+$K$7</x:f>
-        <x:v>DOL</x:v>
+        <x:v>SOL</x:v>
       </x:c>
       <x:c r="J90" s="35"/>
       <x:c r="K90" s="43"/>

</xml_diff>